<commit_message>
finished test client file
</commit_message>
<xml_diff>
--- a/isd_project_harshdeep/tests/A01_pixell_test_plan_client.xlsx
+++ b/isd_project_harshdeep/tests/A01_pixell_test_plan_client.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\OneDrive\Desktop\Documents\rrc-ploytech\semi-2\ISD 2327 assignments\Assignment_1_harshdeep_bhinder\isd_project\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\OneDrive\Desktop\Documents\rrc-ploytech\semi-2\ISD 2327 assignments\Assignment_1_harshdeep_bhinder\isd_project_harshdeep\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6E31C9-6607-4263-BE33-93E3818151A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEC6DE4-5B4C-46BD-A99D-8AA0BC55FEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="1248" yWindow="1248" windowWidth="21600" windowHeight="11292" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1087,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>

</xml_diff>